<commit_message>
refactor biases again (to handle some indecies)
</commit_message>
<xml_diff>
--- a/fflayers_bias.xlsx
+++ b/fflayers_bias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hp\go\src\cnns_vika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6A318E-B48D-4212-B522-40C7600F95CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B89B22-26CE-46F5-92B7-5C9C7EEF3014}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,10 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -572,11 +572,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -598,38 +598,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -715,21 +715,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -768,21 +768,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -815,21 +815,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -873,21 +873,21 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -922,11 +922,11 @@
       <c r="L27" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -1310,6 +1310,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -1317,19 +1330,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1363,11 +1363,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -1389,38 +1389,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1531,21 +1531,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1584,21 +1584,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1631,21 +1631,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1689,21 +1689,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1737,11 +1737,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -2125,6 +2125,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -2132,19 +2145,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2178,11 +2178,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -2204,38 +2204,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -2346,21 +2346,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2399,21 +2399,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2446,21 +2446,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -2504,21 +2504,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -2552,11 +2552,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -2940,6 +2940,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -2947,19 +2960,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2993,11 +2993,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -3019,38 +3019,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -3161,21 +3161,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -3214,21 +3214,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -3261,21 +3261,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -3319,21 +3319,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -3367,11 +3367,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -3755,6 +3755,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -3762,19 +3775,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3808,11 +3808,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -3834,38 +3834,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -3976,21 +3976,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -4029,21 +4029,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -4076,21 +4076,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -4134,21 +4134,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -4182,11 +4182,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -4570,6 +4570,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -4577,19 +4590,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4623,11 +4623,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -4649,38 +4649,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -4791,21 +4791,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -4844,21 +4844,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -4891,21 +4891,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -4949,21 +4949,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -4997,11 +4997,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -5385,6 +5385,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -5392,19 +5405,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5438,11 +5438,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -5464,38 +5464,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -5606,21 +5606,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -5659,21 +5659,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -5706,21 +5706,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -5764,21 +5764,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -5812,11 +5812,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -6200,6 +6200,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -6207,19 +6220,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6253,11 +6253,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -6279,38 +6279,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -6421,21 +6421,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -6474,21 +6474,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -6521,21 +6521,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -6579,21 +6579,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -6627,11 +6627,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -7015,6 +7015,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -7022,19 +7035,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7068,11 +7068,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -7094,38 +7094,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -7236,21 +7236,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -7289,21 +7289,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -7336,21 +7336,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -7394,21 +7394,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -7442,11 +7442,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -7830,6 +7830,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -7837,19 +7850,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7883,11 +7883,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -7909,38 +7909,38 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -8051,21 +8051,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -8104,21 +8104,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -8151,21 +8151,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -8209,21 +8209,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -8257,11 +8257,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="E29" t="s">
         <v>18</v>
       </c>
@@ -8645,6 +8645,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:G6"/>
@@ -8652,19 +8665,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
add printing method for sum delta*wegihts
</commit_message>
<xml_diff>
--- a/fflayers_bias.xlsx
+++ b/fflayers_bias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="step 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,7 +1074,7 @@
   </sheetPr>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J49" activeCellId="0" sqref="J49"/>
     </sheetView>
   </sheetViews>
@@ -1883,7 +1883,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>